<commit_message>
CRM Create Entity In progress
</commit_message>
<xml_diff>
--- a/testData/SMS/WF4_Send_SMS_OOF_S_Test.xlsx
+++ b/testData/SMS/WF4_Send_SMS_OOF_S_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="149">
   <si>
     <t>ModuleName</t>
   </si>
@@ -243,9 +243,6 @@
     <t>SMSTemplate_Msg</t>
   </si>
   <si>
-    <t>Hi, Thanks for contacting RSoft. Test Automation ensures quality of the app and maximum test coverage and validation.</t>
-  </si>
-  <si>
     <t>one</t>
   </si>
   <si>
@@ -282,30 +279,9 @@
     <t>EditSales@rsoft.in</t>
   </si>
   <si>
-    <t>8230618709</t>
-  </si>
-  <si>
-    <t>4442809815</t>
-  </si>
-  <si>
-    <t>5069845530</t>
-  </si>
-  <si>
-    <t>0583850615</t>
-  </si>
-  <si>
-    <t>2024-01-08</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>2024-01-08 02:06:48 PM</t>
-  </si>
-  <si>
-    <t>2024-01-08 02:14:54 PM</t>
-  </si>
-  <si>
     <t>Add New Text</t>
   </si>
   <si>
@@ -447,274 +423,52 @@
     <t>Lead about MobileApp</t>
   </si>
   <si>
-    <t>3054496971</t>
-  </si>
-  <si>
-    <t>7570043976</t>
-  </si>
-  <si>
-    <t>2953743365</t>
-  </si>
-  <si>
-    <t>4976436726</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>2024-01-23</t>
-  </si>
-  <si>
-    <t>2024-01-23 12:54:52 PM</t>
-  </si>
-  <si>
-    <t>2024-01-23 01:03:53 PM</t>
-  </si>
-  <si>
-    <t>2089314263</t>
-  </si>
-  <si>
-    <t>6817654930</t>
-  </si>
-  <si>
-    <t>9975749296</t>
-  </si>
-  <si>
-    <t>4262667725</t>
-  </si>
-  <si>
-    <t>9523249659</t>
-  </si>
-  <si>
-    <t>4143219354</t>
-  </si>
-  <si>
-    <t>7854316613</t>
-  </si>
-  <si>
-    <t>0306452229</t>
-  </si>
-  <si>
-    <t>2269141644</t>
-  </si>
-  <si>
-    <t>5352129046</t>
-  </si>
-  <si>
-    <t>6710902693</t>
-  </si>
-  <si>
-    <t>5753084715</t>
-  </si>
-  <si>
-    <t>7581686750</t>
-  </si>
-  <si>
-    <t>0734638139</t>
-  </si>
-  <si>
-    <t>6093294828</t>
-  </si>
-  <si>
-    <t>4849348212</t>
-  </si>
-  <si>
-    <t>2024-01-23 02:50:42 PM</t>
-  </si>
-  <si>
-    <t>2024-01-23 02:58:00 PM</t>
-  </si>
-  <si>
-    <t>0320731177</t>
-  </si>
-  <si>
-    <t>3723286554</t>
-  </si>
-  <si>
-    <t>0107516670</t>
-  </si>
-  <si>
-    <t>2307242326</t>
-  </si>
-  <si>
-    <t>2024-02-16</t>
-  </si>
-  <si>
-    <t>2024-02-16 10:45:02 AM</t>
-  </si>
-  <si>
-    <t>3383547892</t>
-  </si>
-  <si>
-    <t>5549313496</t>
-  </si>
-  <si>
-    <t>4410137311</t>
-  </si>
-  <si>
-    <t>1607182956</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:05:20 AM</t>
-  </si>
-  <si>
-    <t>3079717578</t>
-  </si>
-  <si>
-    <t>4302668826</t>
-  </si>
-  <si>
-    <t>1088188534</t>
-  </si>
-  <si>
-    <t>0147255501</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:14:56 AM</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:21:21 AM</t>
-  </si>
-  <si>
-    <t>6662063602</t>
-  </si>
-  <si>
-    <t>1304060830</t>
-  </si>
-  <si>
-    <t>9289789879</t>
-  </si>
-  <si>
-    <t>0473748842</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:35:21 AM</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:41:51 AM</t>
-  </si>
-  <si>
-    <t>6442762697</t>
-  </si>
-  <si>
-    <t>1863802921</t>
-  </si>
-  <si>
-    <t>5569233801</t>
-  </si>
-  <si>
-    <t>6376014794</t>
-  </si>
-  <si>
-    <t>2024-02-16 11:55:33 AM</t>
-  </si>
-  <si>
-    <t>2024-02-16 12:02:04 PM</t>
-  </si>
-  <si>
-    <t>6144307828</t>
-  </si>
-  <si>
-    <t>3999133860</t>
-  </si>
-  <si>
-    <t>7838841250</t>
-  </si>
-  <si>
-    <t>0071638138</t>
-  </si>
-  <si>
-    <t>1982503987</t>
-  </si>
-  <si>
-    <t>5041238076</t>
-  </si>
-  <si>
-    <t>5608599758</t>
-  </si>
-  <si>
-    <t>4337605175</t>
-  </si>
-  <si>
-    <t>4636768556</t>
-  </si>
-  <si>
-    <t>5731752431</t>
-  </si>
-  <si>
-    <t>5131757743</t>
-  </si>
-  <si>
-    <t>2500787745</t>
-  </si>
-  <si>
-    <t>5938415728</t>
-  </si>
-  <si>
-    <t>0352373990</t>
-  </si>
-  <si>
-    <t>8698287359</t>
-  </si>
-  <si>
-    <t>3333757687</t>
-  </si>
-  <si>
-    <t>7750779274</t>
-  </si>
-  <si>
-    <t>1227554203</t>
-  </si>
-  <si>
-    <t>2315389233</t>
-  </si>
-  <si>
-    <t>8951998491</t>
-  </si>
-  <si>
-    <t>0154261887</t>
-  </si>
-  <si>
-    <t>4513506486</t>
-  </si>
-  <si>
-    <t>8490656755</t>
-  </si>
-  <si>
-    <t>6963187389</t>
-  </si>
-  <si>
-    <t>6035641181</t>
-  </si>
-  <si>
-    <t>3025930051</t>
-  </si>
-  <si>
-    <t>1866622516</t>
-  </si>
-  <si>
-    <t>3087938090</t>
-  </si>
-  <si>
-    <t>9913527335</t>
-  </si>
-  <si>
-    <t>1359624562</t>
-  </si>
-  <si>
-    <t>4951701364</t>
-  </si>
-  <si>
-    <t>4612685582</t>
-  </si>
-  <si>
-    <t>2024-02-21</t>
-  </si>
-  <si>
-    <t>2024-02-21 11:15:53 AM</t>
-  </si>
-  <si>
-    <t>2024-02-21 11:24:08 AM</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2024-03-06</t>
+  </si>
+  <si>
+    <t>CurrentTime</t>
+  </si>
+  <si>
+    <t>2024-03-06 01:44:34 PM</t>
+  </si>
+  <si>
+    <t>CT. Wed, Mar 06, 2024 at 1:49 PM</t>
+  </si>
+  <si>
+    <t>2024-03-06 01:52:14 PM</t>
+  </si>
+  <si>
+    <t>CT. Wed, Mar 06, 2024 at 1:57 PM</t>
+  </si>
+  <si>
+    <t>CT. Wed, Mar 06, 2024 at 2:05 PM</t>
+  </si>
+  <si>
+    <t>4324529975</t>
+  </si>
+  <si>
+    <t>4009429147</t>
+  </si>
+  <si>
+    <t>4518943107</t>
+  </si>
+  <si>
+    <t>2819678667</t>
+  </si>
+  <si>
+    <t>7571439520</t>
+  </si>
+  <si>
+    <t>8441366716</t>
+  </si>
+  <si>
+    <t>4726587529</t>
+  </si>
+  <si>
+    <t>2297189724</t>
   </si>
 </sst>
 </file>
@@ -1061,7 +815,7 @@
   <dimension ref="A1:AZ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1110,8 +864,8 @@
     <col min="48" max="48" bestFit="true" customWidth="true" style="2" width="10.90625"/>
     <col min="49" max="49" bestFit="true" customWidth="true" style="2" width="14.08984375"/>
     <col min="50" max="50" bestFit="true" customWidth="true" style="2" width="10.81640625"/>
-    <col min="51" max="51" customWidth="true" style="2" width="10.36328125"/>
-    <col min="52" max="52" customWidth="true" style="2" width="25.81640625"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" style="2" width="22.7265625"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="2" width="30.26953125"/>
     <col min="53" max="16384" style="2" width="8.7265625"/>
   </cols>
   <sheetData>
@@ -1270,7 +1024,7 @@
         <v>61</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="72.5" x14ac:dyDescent="0.35">
@@ -1284,22 +1038,22 @@
         <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H2" s="2">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>23</v>
@@ -1313,14 +1067,14 @@
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>229</v>
+      <c r="N2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="Q2" s="2">
         <v>444444444</v>
@@ -1332,7 +1086,7 @@
         <v>38</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U2" s="2">
         <v>11111111111</v>
@@ -1347,25 +1101,25 @@
         <v>50</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s" s="2">
-        <v>228</v>
+      <c r="AC2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>225</v>
+        <v>146</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>41</v>
@@ -1380,7 +1134,7 @@
         <v>67</v>
       </c>
       <c r="AK2" t="s" s="2">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="AQ2" s="2" t="s">
         <v>51</v>
@@ -1392,25 +1146,25 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>226</v>
+        <v>147</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="AW2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>227</v>
+        <v>148</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>73</v>
+        <v>94</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1640,7 +1394,7 @@
         <v>61</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="116" x14ac:dyDescent="0.35">
@@ -1654,43 +1408,43 @@
         <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="H2" s="2">
         <v>4</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>230</v>
+        <v>100</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="Q2" s="2">
         <v>55555555555</v>
@@ -1702,7 +1456,7 @@
         <v>50</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="U2" s="2">
         <v>44444444444</v>
@@ -1711,31 +1465,31 @@
         <v>20000</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s" s="2">
-        <v>228</v>
+      <c r="AC2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>225</v>
+        <v>146</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>41</v>
@@ -1759,25 +1513,25 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>226</v>
+        <v>147</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="AW2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>227</v>
+        <v>148</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>76</v>
+        <v>109</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2013,43 +1767,43 @@
         <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="H2" s="2">
         <v>3</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>230</v>
+      <c r="N2" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="Q2" s="2">
         <v>666666666</v>
@@ -2058,10 +1812,10 @@
         <v>45</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="U2" s="2">
         <v>33333333333</v>
@@ -2070,34 +1824,34 @@
         <v>8000</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s" s="2">
-        <v>171</v>
+      <c r="AC2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>225</v>
+        <v>146</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>68</v>
@@ -2118,25 +1872,25 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>226</v>
+        <v>147</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="AW2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>227</v>
+        <v>148</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2358,7 +2112,7 @@
         <v>61</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="116" x14ac:dyDescent="0.35">
@@ -2372,43 +2126,43 @@
         <v>44</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H2" s="2">
         <v>5</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="L2" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="M2" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="N2" t="s" s="2">
-        <v>171</v>
-      </c>
-      <c r="O2" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="P2" t="s" s="2">
-        <v>195</v>
+      <c r="O2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="Q2" s="2">
         <v>7777777777</v>
@@ -2417,10 +2171,10 @@
         <v>45</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="U2" s="2">
         <v>6666666666</v>
@@ -2429,34 +2183,34 @@
         <v>40000</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="X2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="Z2" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" t="s" s="2">
-        <v>171</v>
+      <c r="AC2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>225</v>
+        <v>146</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>68</v>
@@ -2477,25 +2231,25 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>226</v>
+        <v>147</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="AW2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>227</v>
+        <v>148</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="AZ2" s="1" t="s">
-        <v>76</v>
+        <v>84</v>
+      </c>
+      <c r="AZ2" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SMS Scripts dry run
</commit_message>
<xml_diff>
--- a/testData/SMS/WF4_Send_SMS_OOF_S_Test.xlsx
+++ b/testData/SMS/WF4_Send_SMS_OOF_S_Test.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="190">
   <si>
     <t>ModuleName</t>
   </si>
@@ -475,6 +475,123 @@
   </si>
   <si>
     <t>5501425979</t>
+  </si>
+  <si>
+    <t>5323798946</t>
+  </si>
+  <si>
+    <t>1486540809</t>
+  </si>
+  <si>
+    <t>8429199210</t>
+  </si>
+  <si>
+    <t>4740651754</t>
+  </si>
+  <si>
+    <t>5827216557</t>
+  </si>
+  <si>
+    <t>5290040062</t>
+  </si>
+  <si>
+    <t>2992827932</t>
+  </si>
+  <si>
+    <t>4951577755</t>
+  </si>
+  <si>
+    <t>2478144177</t>
+  </si>
+  <si>
+    <t>3112188866</t>
+  </si>
+  <si>
+    <t>1074500286</t>
+  </si>
+  <si>
+    <t>0547819386</t>
+  </si>
+  <si>
+    <t>2024-05-25</t>
+  </si>
+  <si>
+    <t>02:35:55 AM</t>
+  </si>
+  <si>
+    <t>2024-04-28 05:00:00 PM</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 11:18 AM</t>
+  </si>
+  <si>
+    <t>6807832171</t>
+  </si>
+  <si>
+    <t>9665637567</t>
+  </si>
+  <si>
+    <t>4298629953</t>
+  </si>
+  <si>
+    <t>9126802701</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 11:35 AM</t>
+  </si>
+  <si>
+    <t>9120414700</t>
+  </si>
+  <si>
+    <t>3321774125</t>
+  </si>
+  <si>
+    <t>0457006885</t>
+  </si>
+  <si>
+    <t>4447502254</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 11:47 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 11:55 AM</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 12:04 PM</t>
+  </si>
+  <si>
+    <t>0305177807</t>
+  </si>
+  <si>
+    <t>5725131934</t>
+  </si>
+  <si>
+    <t>8611387896</t>
+  </si>
+  <si>
+    <t>0374289525</t>
+  </si>
+  <si>
+    <t>0286115958</t>
+  </si>
+  <si>
+    <t>3049192532</t>
+  </si>
+  <si>
+    <t>5178268986</t>
+  </si>
+  <si>
+    <t>8330429640</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 12:48 PM</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 12:56 PM</t>
+  </si>
+  <si>
+    <t>CT: Sat, May 25, 2024 at 1:05 PM</t>
   </si>
 </sst>
 </file>
@@ -1050,7 +1167,7 @@
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>87</v>
@@ -1073,14 +1190,14 @@
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="N2" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>140</v>
+      <c r="P2" t="s" s="2">
+        <v>165</v>
       </c>
       <c r="Q2" s="2">
         <v>444444444</v>
@@ -1118,14 +1235,14 @@
       <c r="AB2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>138</v>
+      <c r="AC2" t="s" s="2">
+        <v>163</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>41</v>
@@ -1152,7 +1269,7 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>92</v>
@@ -1164,13 +1281,13 @@
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="AY2" s="4" t="s">
         <v>94</v>
       </c>
       <c r="AZ2" t="s" s="2">
-        <v>146</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -1399,7 +1516,7 @@
       <c r="AY1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" t="s" s="2">
         <v>134</v>
       </c>
     </row>
@@ -1420,7 +1537,7 @@
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>96</v>
@@ -1443,14 +1560,14 @@
       <c r="M2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="O2" s="2" t="s">
+      <c r="N2" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>140</v>
+      <c r="P2" t="s" s="2">
+        <v>165</v>
       </c>
       <c r="Q2" s="2">
         <v>55555555555</v>
@@ -1488,14 +1605,14 @@
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>138</v>
+      <c r="AC2" t="s" s="2">
+        <v>163</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>41</v>
@@ -1519,7 +1636,7 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>107</v>
@@ -1531,13 +1648,13 @@
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="AY2" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="AZ2" s="2" t="s">
-        <v>146</v>
+      <c r="AZ2" t="s" s="2">
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1758,8 +1875,8 @@
       <c r="AY1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AZ1" s="2" t="s">
-        <v>72</v>
+      <c r="AZ1" t="s" s="2">
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:52" ht="116" x14ac:dyDescent="0.35">
@@ -1779,7 +1896,7 @@
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>111</v>
@@ -1802,14 +1919,14 @@
       <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>135</v>
+      <c r="N2" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="P2" t="s" s="2">
+        <v>165</v>
       </c>
       <c r="Q2" s="2">
         <v>666666666</v>
@@ -1847,14 +1964,14 @@
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>133</v>
+      <c r="AC2" t="s" s="2">
+        <v>163</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>78</v>
@@ -1878,7 +1995,7 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>121</v>
@@ -1890,13 +2007,13 @@
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="AY2" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="AZ2" s="1" t="s">
-        <v>75</v>
+      <c r="AZ2" t="s" s="2">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2117,7 +2234,7 @@
       <c r="AY1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="AZ1" t="s" s="2">
         <v>134</v>
       </c>
     </row>
@@ -2138,7 +2255,7 @@
         <v>42</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>79</v>
@@ -2161,14 +2278,14 @@
       <c r="M2" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="N2" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>135</v>
+      <c r="N2" t="s" s="2">
+        <v>163</v>
+      </c>
+      <c r="O2" t="s" s="2">
+        <v>139</v>
+      </c>
+      <c r="P2" t="s" s="2">
+        <v>165</v>
       </c>
       <c r="Q2" s="2">
         <v>7777777777</v>
@@ -2206,14 +2323,14 @@
       <c r="AB2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AC2" s="2" t="s">
-        <v>133</v>
+      <c r="AC2" t="s" s="2">
+        <v>163</v>
       </c>
       <c r="AD2" s="3" t="s">
         <v>43</v>
       </c>
       <c r="AE2" t="s" s="2">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="AF2" s="2" t="s">
         <v>91</v>
@@ -2237,7 +2354,7 @@
         <v>63</v>
       </c>
       <c r="AT2" t="s" s="2">
-        <v>149</v>
+        <v>185</v>
       </c>
       <c r="AU2" s="4" t="s">
         <v>83</v>
@@ -2249,13 +2366,13 @@
         <v>43</v>
       </c>
       <c r="AX2" t="s" s="2">
-        <v>150</v>
+        <v>186</v>
       </c>
       <c r="AY2" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="AZ2" s="2" t="s">
-        <v>136</v>
+      <c r="AZ2" t="s" s="2">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>